<commit_message>
separation of concerns, added AE questions
</commit_message>
<xml_diff>
--- a/output/CCA SFO Chinese_Processed_2024-11-14.xlsx
+++ b/output/CCA SFO Chinese_Processed_2024-11-14.xlsx
@@ -1237,8 +1237,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B2" s="21" t="n">
-        <v>45617</v>
+      <c r="B2" s="21" t="inlineStr">
+        <is>
+          <t>11/21/2024</t>
+        </is>
       </c>
       <c r="C2" s="22">
         <f>B2</f>
@@ -1329,7 +1331,7 @@
       </c>
       <c r="Y2" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z2" s="6" t="inlineStr">
@@ -1357,8 +1359,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B3" s="21" t="n">
-        <v>45616</v>
+      <c r="B3" s="21" t="inlineStr">
+        <is>
+          <t>11/20/2024</t>
+        </is>
       </c>
       <c r="C3" s="22">
         <f>B3</f>
@@ -1449,7 +1453,7 @@
       </c>
       <c r="Y3" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z3" s="6" t="inlineStr">
@@ -1477,8 +1481,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B4" s="21" t="n">
-        <v>45615</v>
+      <c r="B4" s="21" t="inlineStr">
+        <is>
+          <t>11/19/2024</t>
+        </is>
       </c>
       <c r="C4" s="22">
         <f>B4</f>
@@ -1569,7 +1575,7 @@
       </c>
       <c r="Y4" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z4" s="6" t="inlineStr">
@@ -1597,8 +1603,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B5" s="21" t="n">
-        <v>45620</v>
+      <c r="B5" s="21" t="inlineStr">
+        <is>
+          <t>11/24/2024</t>
+        </is>
       </c>
       <c r="C5" s="22">
         <f>B5</f>
@@ -1689,7 +1697,7 @@
       </c>
       <c r="Y5" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z5" s="6" t="inlineStr">
@@ -1717,8 +1725,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B6" s="21" t="n">
-        <v>45619</v>
+      <c r="B6" s="21" t="inlineStr">
+        <is>
+          <t>11/23/2024</t>
+        </is>
       </c>
       <c r="C6" s="22">
         <f>B6</f>
@@ -1809,7 +1819,7 @@
       </c>
       <c r="Y6" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z6" s="6" t="inlineStr">
@@ -1837,8 +1847,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B7" s="21" t="n">
-        <v>45618</v>
+      <c r="B7" s="21" t="inlineStr">
+        <is>
+          <t>11/22/2024</t>
+        </is>
       </c>
       <c r="C7" s="22">
         <f>B7</f>
@@ -1929,7 +1941,7 @@
       </c>
       <c r="Y7" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z7" s="6" t="inlineStr">
@@ -1957,8 +1969,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B8" s="21" t="n">
-        <v>45633</v>
+      <c r="B8" s="21" t="inlineStr">
+        <is>
+          <t>12/7/2024</t>
+        </is>
       </c>
       <c r="C8" s="22">
         <f>B8</f>
@@ -2049,7 +2063,7 @@
       </c>
       <c r="Y8" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z8" s="6" t="inlineStr">
@@ -2077,8 +2091,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B9" s="21" t="n">
-        <v>45628</v>
+      <c r="B9" s="21" t="inlineStr">
+        <is>
+          <t>12/2/2024</t>
+        </is>
       </c>
       <c r="C9" s="22">
         <f>B9</f>
@@ -2169,7 +2185,7 @@
       </c>
       <c r="Y9" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z9" s="6" t="inlineStr">
@@ -2197,8 +2213,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B10" s="21" t="n">
-        <v>45630</v>
+      <c r="B10" s="21" t="inlineStr">
+        <is>
+          <t>12/4/2024</t>
+        </is>
       </c>
       <c r="C10" s="22">
         <f>B10</f>
@@ -2289,7 +2307,7 @@
       </c>
       <c r="Y10" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z10" s="6" t="inlineStr">
@@ -2317,8 +2335,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B11" s="21" t="n">
-        <v>45632</v>
+      <c r="B11" s="21" t="inlineStr">
+        <is>
+          <t>12/6/2024</t>
+        </is>
       </c>
       <c r="C11" s="22">
         <f>B11</f>
@@ -2409,7 +2429,7 @@
       </c>
       <c r="Y11" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z11" s="6" t="inlineStr">
@@ -2437,8 +2457,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B12" s="21" t="n">
-        <v>45629</v>
+      <c r="B12" s="21" t="inlineStr">
+        <is>
+          <t>12/3/2024</t>
+        </is>
       </c>
       <c r="C12" s="22">
         <f>B12</f>
@@ -2529,7 +2551,7 @@
       </c>
       <c r="Y12" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z12" s="6" t="inlineStr">
@@ -2557,8 +2579,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B13" s="21" t="n">
-        <v>45631</v>
+      <c r="B13" s="21" t="inlineStr">
+        <is>
+          <t>12/5/2024</t>
+        </is>
       </c>
       <c r="C13" s="22">
         <f>B13</f>
@@ -2649,7 +2673,7 @@
       </c>
       <c r="Y13" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z13" s="6" t="inlineStr">
@@ -2677,8 +2701,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B14" s="21" t="n">
-        <v>45638</v>
+      <c r="B14" s="21" t="inlineStr">
+        <is>
+          <t>12/12/2024</t>
+        </is>
       </c>
       <c r="C14" s="22">
         <f>B14</f>
@@ -2769,7 +2795,7 @@
       </c>
       <c r="Y14" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z14" s="6" t="inlineStr">
@@ -2797,8 +2823,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B15" s="21" t="n">
-        <v>45638</v>
+      <c r="B15" s="21" t="inlineStr">
+        <is>
+          <t>12/12/2024</t>
+        </is>
       </c>
       <c r="C15" s="22">
         <f>B15</f>
@@ -2889,7 +2917,7 @@
       </c>
       <c r="Y15" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z15" s="6" t="inlineStr">
@@ -2917,8 +2945,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B16" s="21" t="n">
-        <v>45636</v>
+      <c r="B16" s="21" t="inlineStr">
+        <is>
+          <t>12/10/2024</t>
+        </is>
       </c>
       <c r="C16" s="22">
         <f>B16</f>
@@ -3009,7 +3039,7 @@
       </c>
       <c r="Y16" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z16" s="6" t="inlineStr">
@@ -3037,8 +3067,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B17" s="21" t="n">
-        <v>45639</v>
+      <c r="B17" s="21" t="inlineStr">
+        <is>
+          <t>12/13/2024</t>
+        </is>
       </c>
       <c r="C17" s="22">
         <f>B17</f>
@@ -3129,7 +3161,7 @@
       </c>
       <c r="Y17" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z17" s="6" t="inlineStr">
@@ -3157,8 +3189,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B18" s="21" t="n">
-        <v>45641</v>
+      <c r="B18" s="21" t="inlineStr">
+        <is>
+          <t>12/15/2024</t>
+        </is>
       </c>
       <c r="C18" s="22">
         <f>B18</f>
@@ -3249,7 +3283,7 @@
       </c>
       <c r="Y18" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z18" s="6" t="inlineStr">
@@ -3277,8 +3311,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B19" s="21" t="n">
-        <v>45639</v>
+      <c r="B19" s="21" t="inlineStr">
+        <is>
+          <t>12/13/2024</t>
+        </is>
       </c>
       <c r="C19" s="22">
         <f>B19</f>
@@ -3369,7 +3405,7 @@
       </c>
       <c r="Y19" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z19" s="6" t="inlineStr">
@@ -3397,8 +3433,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B20" s="21" t="n">
-        <v>45635</v>
+      <c r="B20" s="21" t="inlineStr">
+        <is>
+          <t>12/9/2024</t>
+        </is>
       </c>
       <c r="C20" s="22">
         <f>B20</f>
@@ -3489,7 +3527,7 @@
       </c>
       <c r="Y20" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z20" s="6" t="inlineStr">
@@ -3517,8 +3555,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B21" s="21" t="n">
-        <v>45636</v>
+      <c r="B21" s="21" t="inlineStr">
+        <is>
+          <t>12/10/2024</t>
+        </is>
       </c>
       <c r="C21" s="22">
         <f>B21</f>
@@ -3609,7 +3649,7 @@
       </c>
       <c r="Y21" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z21" s="6" t="inlineStr">
@@ -3637,8 +3677,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B22" s="21" t="n">
-        <v>45641</v>
+      <c r="B22" s="21" t="inlineStr">
+        <is>
+          <t>12/15/2024</t>
+        </is>
       </c>
       <c r="C22" s="22">
         <f>B22</f>
@@ -3729,7 +3771,7 @@
       </c>
       <c r="Y22" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z22" s="6" t="inlineStr">
@@ -3757,8 +3799,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B23" s="21" t="n">
-        <v>45635</v>
+      <c r="B23" s="21" t="inlineStr">
+        <is>
+          <t>12/9/2024</t>
+        </is>
       </c>
       <c r="C23" s="22">
         <f>B23</f>
@@ -3849,7 +3893,7 @@
       </c>
       <c r="Y23" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z23" s="6" t="inlineStr">
@@ -3877,8 +3921,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B24" s="21" t="n">
-        <v>45644</v>
+      <c r="B24" s="21" t="inlineStr">
+        <is>
+          <t>12/18/2024</t>
+        </is>
       </c>
       <c r="C24" s="22">
         <f>B24</f>
@@ -3969,7 +4015,7 @@
       </c>
       <c r="Y24" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z24" s="6" t="inlineStr">
@@ -3997,8 +4043,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B25" s="21" t="n">
-        <v>45645</v>
+      <c r="B25" s="21" t="inlineStr">
+        <is>
+          <t>12/19/2024</t>
+        </is>
       </c>
       <c r="C25" s="22">
         <f>B25</f>
@@ -4089,7 +4137,7 @@
       </c>
       <c r="Y25" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z25" s="6" t="inlineStr">
@@ -4117,8 +4165,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B26" s="21" t="n">
-        <v>45646</v>
+      <c r="B26" s="21" t="inlineStr">
+        <is>
+          <t>12/20/2024</t>
+        </is>
       </c>
       <c r="C26" s="22">
         <f>B26</f>
@@ -4209,7 +4259,7 @@
       </c>
       <c r="Y26" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z26" s="6" t="inlineStr">
@@ -4237,8 +4287,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B27" s="21" t="n">
-        <v>45648</v>
+      <c r="B27" s="21" t="inlineStr">
+        <is>
+          <t>12/22/2024</t>
+        </is>
       </c>
       <c r="C27" s="22">
         <f>B27</f>
@@ -4329,7 +4381,7 @@
       </c>
       <c r="Y27" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z27" s="6" t="inlineStr">
@@ -4357,8 +4409,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B28" s="21" t="n">
-        <v>45646</v>
+      <c r="B28" s="21" t="inlineStr">
+        <is>
+          <t>12/20/2024</t>
+        </is>
       </c>
       <c r="C28" s="22">
         <f>B28</f>
@@ -4449,7 +4503,7 @@
       </c>
       <c r="Y28" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z28" s="6" t="inlineStr">
@@ -4477,8 +4531,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B29" s="21" t="n">
-        <v>45645</v>
+      <c r="B29" s="21" t="inlineStr">
+        <is>
+          <t>12/19/2024</t>
+        </is>
       </c>
       <c r="C29" s="22">
         <f>B29</f>
@@ -4569,7 +4625,7 @@
       </c>
       <c r="Y29" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z29" s="6" t="inlineStr">
@@ -4597,8 +4653,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B30" s="21" t="n">
-        <v>45642</v>
+      <c r="B30" s="21" t="inlineStr">
+        <is>
+          <t>12/16/2024</t>
+        </is>
       </c>
       <c r="C30" s="22">
         <f>B30</f>
@@ -4689,7 +4747,7 @@
       </c>
       <c r="Y30" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z30" s="6" t="inlineStr">
@@ -4717,8 +4775,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B31" s="21" t="n">
-        <v>45648</v>
+      <c r="B31" s="21" t="inlineStr">
+        <is>
+          <t>12/22/2024</t>
+        </is>
       </c>
       <c r="C31" s="22">
         <f>B31</f>
@@ -4809,7 +4869,7 @@
       </c>
       <c r="Y31" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z31" s="6" t="inlineStr">
@@ -4837,8 +4897,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B32" s="21" t="n">
-        <v>45642</v>
+      <c r="B32" s="21" t="inlineStr">
+        <is>
+          <t>12/16/2024</t>
+        </is>
       </c>
       <c r="C32" s="22">
         <f>B32</f>
@@ -4929,7 +4991,7 @@
       </c>
       <c r="Y32" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z32" s="6" t="inlineStr">
@@ -4957,8 +5019,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B33" s="21" t="n">
-        <v>45644</v>
+      <c r="B33" s="21" t="inlineStr">
+        <is>
+          <t>12/18/2024</t>
+        </is>
       </c>
       <c r="C33" s="22">
         <f>B33</f>
@@ -5049,7 +5113,7 @@
       </c>
       <c r="Y33" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z33" s="6" t="inlineStr">
@@ -5077,8 +5141,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B34" s="21" t="n">
-        <v>45653</v>
+      <c r="B34" s="21" t="inlineStr">
+        <is>
+          <t>12/27/2024</t>
+        </is>
       </c>
       <c r="C34" s="22">
         <f>B34</f>
@@ -5169,7 +5235,7 @@
       </c>
       <c r="Y34" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z34" s="6" t="inlineStr">
@@ -5197,8 +5263,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B35" s="21" t="n">
-        <v>45649</v>
+      <c r="B35" s="21" t="inlineStr">
+        <is>
+          <t>12/23/2024</t>
+        </is>
       </c>
       <c r="C35" s="22">
         <f>B35</f>
@@ -5289,7 +5357,7 @@
       </c>
       <c r="Y35" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z35" s="6" t="inlineStr">
@@ -5317,8 +5385,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B36" s="21" t="n">
-        <v>45654</v>
+      <c r="B36" s="21" t="inlineStr">
+        <is>
+          <t>12/28/2024</t>
+        </is>
       </c>
       <c r="C36" s="22">
         <f>B36</f>
@@ -5409,7 +5479,7 @@
       </c>
       <c r="Y36" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z36" s="6" t="inlineStr">
@@ -5437,8 +5507,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B37" s="21" t="n">
-        <v>45652</v>
+      <c r="B37" s="21" t="inlineStr">
+        <is>
+          <t>12/26/2024</t>
+        </is>
       </c>
       <c r="C37" s="22">
         <f>B37</f>
@@ -5529,7 +5601,7 @@
       </c>
       <c r="Y37" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z37" s="6" t="inlineStr">
@@ -5557,8 +5629,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B38" s="21" t="n">
-        <v>45653</v>
+      <c r="B38" s="21" t="inlineStr">
+        <is>
+          <t>12/27/2024</t>
+        </is>
       </c>
       <c r="C38" s="22">
         <f>B38</f>
@@ -5649,7 +5723,7 @@
       </c>
       <c r="Y38" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z38" s="6" t="inlineStr">
@@ -5677,8 +5751,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B39" s="21" t="n">
-        <v>45654</v>
+      <c r="B39" s="21" t="inlineStr">
+        <is>
+          <t>12/28/2024</t>
+        </is>
       </c>
       <c r="C39" s="22">
         <f>B39</f>
@@ -5769,7 +5845,7 @@
       </c>
       <c r="Y39" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z39" s="6" t="inlineStr">
@@ -5797,8 +5873,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B40" s="21" t="n">
-        <v>45649</v>
+      <c r="B40" s="21" t="inlineStr">
+        <is>
+          <t>12/23/2024</t>
+        </is>
       </c>
       <c r="C40" s="22">
         <f>B40</f>
@@ -5889,7 +5967,7 @@
       </c>
       <c r="Y40" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z40" s="6" t="inlineStr">
@@ -5917,8 +5995,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B41" s="21" t="n">
-        <v>45655</v>
+      <c r="B41" s="21" t="inlineStr">
+        <is>
+          <t>12/29/2024</t>
+        </is>
       </c>
       <c r="C41" s="22">
         <f>B41</f>
@@ -6009,7 +6089,7 @@
       </c>
       <c r="Y41" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z41" s="6" t="inlineStr">
@@ -6037,8 +6117,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B42" s="21" t="n">
-        <v>45652</v>
+      <c r="B42" s="21" t="inlineStr">
+        <is>
+          <t>12/26/2024</t>
+        </is>
       </c>
       <c r="C42" s="22">
         <f>B42</f>
@@ -6129,7 +6211,7 @@
       </c>
       <c r="Y42" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z42" s="6" t="inlineStr">
@@ -6157,8 +6239,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B43" s="21" t="n">
-        <v>45655</v>
+      <c r="B43" s="21" t="inlineStr">
+        <is>
+          <t>12/29/2024</t>
+        </is>
       </c>
       <c r="C43" s="22">
         <f>B43</f>
@@ -6249,7 +6333,7 @@
       </c>
       <c r="Y43" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z43" s="6" t="inlineStr">
@@ -6277,8 +6361,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B44" s="21" t="n">
-        <v>45657</v>
+      <c r="B44" s="21" t="inlineStr">
+        <is>
+          <t>12/31/2024</t>
+        </is>
       </c>
       <c r="C44" s="22">
         <f>B44</f>
@@ -6369,7 +6455,7 @@
       </c>
       <c r="Y44" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z44" s="6" t="inlineStr">
@@ -6397,8 +6483,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B45" s="21" t="n">
-        <v>45656</v>
+      <c r="B45" s="21" t="inlineStr">
+        <is>
+          <t>12/30/2024</t>
+        </is>
       </c>
       <c r="C45" s="22">
         <f>B45</f>
@@ -6489,7 +6577,7 @@
       </c>
       <c r="Y45" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z45" s="6" t="inlineStr">
@@ -6517,8 +6605,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B46" s="21" t="n">
-        <v>45657</v>
+      <c r="B46" s="21" t="inlineStr">
+        <is>
+          <t>12/31/2024</t>
+        </is>
       </c>
       <c r="C46" s="22">
         <f>B46</f>
@@ -6609,7 +6699,7 @@
       </c>
       <c r="Y46" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z46" s="6" t="inlineStr">
@@ -6637,8 +6727,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B47" s="21" t="n">
-        <v>45673</v>
+      <c r="B47" s="21" t="inlineStr">
+        <is>
+          <t>1/16/2025</t>
+        </is>
       </c>
       <c r="C47" s="22">
         <f>B47</f>
@@ -6729,7 +6821,7 @@
       </c>
       <c r="Y47" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z47" s="6" t="inlineStr">
@@ -6757,8 +6849,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B48" s="21" t="n">
-        <v>45676</v>
+      <c r="B48" s="21" t="inlineStr">
+        <is>
+          <t>1/19/2025</t>
+        </is>
       </c>
       <c r="C48" s="22">
         <f>B48</f>
@@ -6849,7 +6943,7 @@
       </c>
       <c r="Y48" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z48" s="6" t="inlineStr">
@@ -6877,8 +6971,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B49" s="21" t="n">
-        <v>45670</v>
+      <c r="B49" s="21" t="inlineStr">
+        <is>
+          <t>1/13/2025</t>
+        </is>
       </c>
       <c r="C49" s="22">
         <f>B49</f>
@@ -6969,7 +7065,7 @@
       </c>
       <c r="Y49" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z49" s="6" t="inlineStr">
@@ -6997,8 +7093,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B50" s="21" t="n">
-        <v>45671</v>
+      <c r="B50" s="21" t="inlineStr">
+        <is>
+          <t>1/14/2025</t>
+        </is>
       </c>
       <c r="C50" s="22">
         <f>B50</f>
@@ -7089,7 +7187,7 @@
       </c>
       <c r="Y50" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z50" s="6" t="inlineStr">
@@ -7117,8 +7215,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B51" s="21" t="n">
-        <v>45674</v>
+      <c r="B51" s="21" t="inlineStr">
+        <is>
+          <t>1/17/2025</t>
+        </is>
       </c>
       <c r="C51" s="22">
         <f>B51</f>
@@ -7209,7 +7309,7 @@
       </c>
       <c r="Y51" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z51" s="6" t="inlineStr">
@@ -7237,8 +7337,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B52" s="21" t="n">
-        <v>45672</v>
+      <c r="B52" s="21" t="inlineStr">
+        <is>
+          <t>1/15/2025</t>
+        </is>
       </c>
       <c r="C52" s="22">
         <f>B52</f>
@@ -7329,7 +7431,7 @@
       </c>
       <c r="Y52" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z52" s="6" t="inlineStr">
@@ -7357,8 +7459,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B53" s="21" t="n">
-        <v>45677</v>
+      <c r="B53" s="21" t="inlineStr">
+        <is>
+          <t>1/20/2025</t>
+        </is>
       </c>
       <c r="C53" s="22">
         <f>B53</f>
@@ -7449,7 +7553,7 @@
       </c>
       <c r="Y53" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z53" s="6" t="inlineStr">
@@ -7477,8 +7581,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B54" s="21" t="n">
-        <v>45680</v>
+      <c r="B54" s="21" t="inlineStr">
+        <is>
+          <t>1/23/2025</t>
+        </is>
       </c>
       <c r="C54" s="22">
         <f>B54</f>
@@ -7569,7 +7675,7 @@
       </c>
       <c r="Y54" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z54" s="6" t="inlineStr">
@@ -7597,8 +7703,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B55" s="21" t="n">
-        <v>45683</v>
+      <c r="B55" s="21" t="inlineStr">
+        <is>
+          <t>1/26/2025</t>
+        </is>
       </c>
       <c r="C55" s="22">
         <f>B55</f>
@@ -7689,7 +7797,7 @@
       </c>
       <c r="Y55" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z55" s="6" t="inlineStr">
@@ -7717,8 +7825,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B56" s="21" t="n">
-        <v>45679</v>
+      <c r="B56" s="21" t="inlineStr">
+        <is>
+          <t>1/22/2025</t>
+        </is>
       </c>
       <c r="C56" s="22">
         <f>B56</f>
@@ -7809,7 +7919,7 @@
       </c>
       <c r="Y56" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z56" s="6" t="inlineStr">
@@ -7837,8 +7947,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B57" s="21" t="n">
-        <v>45680</v>
+      <c r="B57" s="21" t="inlineStr">
+        <is>
+          <t>1/23/2025</t>
+        </is>
       </c>
       <c r="C57" s="22">
         <f>B57</f>
@@ -7929,7 +8041,7 @@
       </c>
       <c r="Y57" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z57" s="6" t="inlineStr">
@@ -7957,8 +8069,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B58" s="21" t="n">
-        <v>45677</v>
+      <c r="B58" s="21" t="inlineStr">
+        <is>
+          <t>1/20/2025</t>
+        </is>
       </c>
       <c r="C58" s="22">
         <f>B58</f>
@@ -8049,7 +8163,7 @@
       </c>
       <c r="Y58" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z58" s="6" t="inlineStr">
@@ -8077,8 +8191,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B59" s="21" t="n">
-        <v>45683</v>
+      <c r="B59" s="21" t="inlineStr">
+        <is>
+          <t>1/26/2025</t>
+        </is>
       </c>
       <c r="C59" s="22">
         <f>B59</f>
@@ -8169,7 +8285,7 @@
       </c>
       <c r="Y59" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z59" s="6" t="inlineStr">
@@ -8197,8 +8313,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B60" s="21" t="n">
-        <v>45682</v>
+      <c r="B60" s="21" t="inlineStr">
+        <is>
+          <t>1/25/2025</t>
+        </is>
       </c>
       <c r="C60" s="22">
         <f>B60</f>
@@ -8289,7 +8407,7 @@
       </c>
       <c r="Y60" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z60" s="6" t="inlineStr">
@@ -8317,8 +8435,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B61" s="21" t="n">
-        <v>45682</v>
+      <c r="B61" s="21" t="inlineStr">
+        <is>
+          <t>1/25/2025</t>
+        </is>
       </c>
       <c r="C61" s="22">
         <f>B61</f>
@@ -8409,7 +8529,7 @@
       </c>
       <c r="Y61" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z61" s="6" t="inlineStr">
@@ -8437,8 +8557,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B62" s="21" t="n">
-        <v>45679</v>
+      <c r="B62" s="21" t="inlineStr">
+        <is>
+          <t>1/22/2025</t>
+        </is>
       </c>
       <c r="C62" s="22">
         <f>B62</f>
@@ -8529,7 +8651,7 @@
       </c>
       <c r="Y62" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z62" s="6" t="inlineStr">
@@ -8557,8 +8679,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B63" s="21" t="n">
-        <v>45687</v>
+      <c r="B63" s="21" t="inlineStr">
+        <is>
+          <t>1/30/2025</t>
+        </is>
       </c>
       <c r="C63" s="22">
         <f>B63</f>
@@ -8649,7 +8773,7 @@
       </c>
       <c r="Y63" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z63" s="6" t="inlineStr">
@@ -8677,8 +8801,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B64" s="21" t="n">
-        <v>45686</v>
+      <c r="B64" s="21" t="inlineStr">
+        <is>
+          <t>1/29/2025</t>
+        </is>
       </c>
       <c r="C64" s="22">
         <f>B64</f>
@@ -8769,7 +8895,7 @@
       </c>
       <c r="Y64" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z64" s="6" t="inlineStr">
@@ -8797,8 +8923,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B65" s="21" t="n">
-        <v>45685</v>
+      <c r="B65" s="21" t="inlineStr">
+        <is>
+          <t>1/28/2025</t>
+        </is>
       </c>
       <c r="C65" s="22">
         <f>B65</f>
@@ -8889,7 +9017,7 @@
       </c>
       <c r="Y65" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z65" s="6" t="inlineStr">
@@ -8917,8 +9045,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B66" s="21" t="n">
-        <v>45687</v>
+      <c r="B66" s="21" t="inlineStr">
+        <is>
+          <t>1/30/2025</t>
+        </is>
       </c>
       <c r="C66" s="22">
         <f>B66</f>
@@ -9009,7 +9139,7 @@
       </c>
       <c r="Y66" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z66" s="6" t="inlineStr">
@@ -9037,8 +9167,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B67" s="21" t="n">
-        <v>45685</v>
+      <c r="B67" s="21" t="inlineStr">
+        <is>
+          <t>1/28/2025</t>
+        </is>
       </c>
       <c r="C67" s="22">
         <f>B67</f>
@@ -9129,7 +9261,7 @@
       </c>
       <c r="Y67" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z67" s="6" t="inlineStr">
@@ -9157,8 +9289,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B68" s="21" t="n">
-        <v>45686</v>
+      <c r="B68" s="21" t="inlineStr">
+        <is>
+          <t>1/29/2025</t>
+        </is>
       </c>
       <c r="C68" s="22">
         <f>B68</f>
@@ -9249,7 +9383,7 @@
       </c>
       <c r="Y68" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z68" s="6" t="inlineStr">
@@ -9277,8 +9411,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B69" s="21" t="n">
-        <v>45615</v>
+      <c r="B69" s="21" t="inlineStr">
+        <is>
+          <t>11/19/2024</t>
+        </is>
       </c>
       <c r="C69" s="22">
         <f>B69</f>
@@ -9369,7 +9505,7 @@
       </c>
       <c r="Y69" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z69" s="6" t="inlineStr">
@@ -9397,8 +9533,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B70" s="21" t="n">
-        <v>45620</v>
+      <c r="B70" s="21" t="inlineStr">
+        <is>
+          <t>11/24/2024</t>
+        </is>
       </c>
       <c r="C70" s="22">
         <f>B70</f>
@@ -9489,7 +9627,7 @@
       </c>
       <c r="Y70" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z70" s="6" t="inlineStr">
@@ -9517,8 +9655,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B71" s="21" t="n">
-        <v>45616</v>
+      <c r="B71" s="21" t="inlineStr">
+        <is>
+          <t>11/20/2024</t>
+        </is>
       </c>
       <c r="C71" s="22">
         <f>B71</f>
@@ -9609,7 +9749,7 @@
       </c>
       <c r="Y71" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z71" s="6" t="inlineStr">
@@ -9637,8 +9777,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B72" s="21" t="n">
-        <v>45631</v>
+      <c r="B72" s="21" t="inlineStr">
+        <is>
+          <t>12/5/2024</t>
+        </is>
       </c>
       <c r="C72" s="22">
         <f>B72</f>
@@ -9729,7 +9871,7 @@
       </c>
       <c r="Y72" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z72" s="6" t="inlineStr">
@@ -9757,8 +9899,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B73" s="21" t="n">
-        <v>45632</v>
+      <c r="B73" s="21" t="inlineStr">
+        <is>
+          <t>12/6/2024</t>
+        </is>
       </c>
       <c r="C73" s="22">
         <f>B73</f>
@@ -9849,7 +9993,7 @@
       </c>
       <c r="Y73" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z73" s="6" t="inlineStr">
@@ -9877,8 +10021,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B74" s="21" t="n">
-        <v>45628</v>
+      <c r="B74" s="21" t="inlineStr">
+        <is>
+          <t>12/2/2024</t>
+        </is>
       </c>
       <c r="C74" s="22">
         <f>B74</f>
@@ -9969,7 +10115,7 @@
       </c>
       <c r="Y74" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z74" s="6" t="inlineStr">
@@ -9997,8 +10143,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B75" s="21" t="n">
-        <v>45636</v>
+      <c r="B75" s="21" t="inlineStr">
+        <is>
+          <t>12/10/2024</t>
+        </is>
       </c>
       <c r="C75" s="22">
         <f>B75</f>
@@ -10089,7 +10237,7 @@
       </c>
       <c r="Y75" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z75" s="6" t="inlineStr">
@@ -10117,8 +10265,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B76" s="21" t="n">
-        <v>45640</v>
+      <c r="B76" s="21" t="inlineStr">
+        <is>
+          <t>12/14/2024</t>
+        </is>
       </c>
       <c r="C76" s="22">
         <f>B76</f>
@@ -10209,7 +10359,7 @@
       </c>
       <c r="Y76" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z76" s="6" t="inlineStr">
@@ -10237,8 +10387,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B77" s="21" t="n">
-        <v>45641</v>
+      <c r="B77" s="21" t="inlineStr">
+        <is>
+          <t>12/15/2024</t>
+        </is>
       </c>
       <c r="C77" s="22">
         <f>B77</f>
@@ -10329,7 +10481,7 @@
       </c>
       <c r="Y77" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z77" s="6" t="inlineStr">
@@ -10357,8 +10509,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B78" s="21" t="n">
-        <v>45644</v>
+      <c r="B78" s="21" t="inlineStr">
+        <is>
+          <t>12/18/2024</t>
+        </is>
       </c>
       <c r="C78" s="22">
         <f>B78</f>
@@ -10449,7 +10603,7 @@
       </c>
       <c r="Y78" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z78" s="6" t="inlineStr">
@@ -10477,8 +10631,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B79" s="21" t="n">
-        <v>45648</v>
+      <c r="B79" s="21" t="inlineStr">
+        <is>
+          <t>12/22/2024</t>
+        </is>
       </c>
       <c r="C79" s="22">
         <f>B79</f>
@@ -10569,7 +10725,7 @@
       </c>
       <c r="Y79" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z79" s="6" t="inlineStr">
@@ -10597,8 +10753,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B80" s="21" t="n">
-        <v>45646</v>
+      <c r="B80" s="21" t="inlineStr">
+        <is>
+          <t>12/20/2024</t>
+        </is>
       </c>
       <c r="C80" s="22">
         <f>B80</f>
@@ -10689,7 +10847,7 @@
       </c>
       <c r="Y80" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z80" s="6" t="inlineStr">
@@ -10717,8 +10875,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B81" s="21" t="n">
-        <v>45653</v>
+      <c r="B81" s="21" t="inlineStr">
+        <is>
+          <t>12/27/2024</t>
+        </is>
       </c>
       <c r="C81" s="22">
         <f>B81</f>
@@ -10809,7 +10969,7 @@
       </c>
       <c r="Y81" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z81" s="6" t="inlineStr">
@@ -10837,8 +10997,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B82" s="21" t="n">
-        <v>45652</v>
+      <c r="B82" s="21" t="inlineStr">
+        <is>
+          <t>12/26/2024</t>
+        </is>
       </c>
       <c r="C82" s="22">
         <f>B82</f>
@@ -10929,7 +11091,7 @@
       </c>
       <c r="Y82" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z82" s="6" t="inlineStr">
@@ -10957,8 +11119,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B83" s="21" t="n">
-        <v>45649</v>
+      <c r="B83" s="21" t="inlineStr">
+        <is>
+          <t>12/23/2024</t>
+        </is>
       </c>
       <c r="C83" s="22">
         <f>B83</f>
@@ -11049,7 +11213,7 @@
       </c>
       <c r="Y83" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z83" s="6" t="inlineStr">
@@ -11077,8 +11241,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B84" s="21" t="n">
-        <v>45657</v>
+      <c r="B84" s="21" t="inlineStr">
+        <is>
+          <t>12/31/2024</t>
+        </is>
       </c>
       <c r="C84" s="22">
         <f>B84</f>
@@ -11169,7 +11335,7 @@
       </c>
       <c r="Y84" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z84" s="6" t="inlineStr">
@@ -11197,8 +11363,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B85" s="21" t="n">
-        <v>45656</v>
+      <c r="B85" s="21" t="inlineStr">
+        <is>
+          <t>12/30/2024</t>
+        </is>
       </c>
       <c r="C85" s="22">
         <f>B85</f>
@@ -11289,7 +11457,7 @@
       </c>
       <c r="Y85" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z85" s="6" t="inlineStr">
@@ -11317,8 +11485,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B86" s="21" t="n">
-        <v>45657</v>
+      <c r="B86" s="21" t="inlineStr">
+        <is>
+          <t>12/31/2024</t>
+        </is>
       </c>
       <c r="C86" s="22">
         <f>B86</f>
@@ -11409,7 +11579,7 @@
       </c>
       <c r="Y86" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z86" s="6" t="inlineStr">
@@ -11437,8 +11607,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B87" s="21" t="n">
-        <v>45672</v>
+      <c r="B87" s="21" t="inlineStr">
+        <is>
+          <t>1/15/2025</t>
+        </is>
       </c>
       <c r="C87" s="22">
         <f>B87</f>
@@ -11529,7 +11701,7 @@
       </c>
       <c r="Y87" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z87" s="6" t="inlineStr">
@@ -11557,8 +11729,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B88" s="21" t="n">
-        <v>45671</v>
+      <c r="B88" s="21" t="inlineStr">
+        <is>
+          <t>1/14/2025</t>
+        </is>
       </c>
       <c r="C88" s="22">
         <f>B88</f>
@@ -11649,7 +11823,7 @@
       </c>
       <c r="Y88" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z88" s="6" t="inlineStr">
@@ -11677,8 +11851,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B89" s="21" t="n">
-        <v>45673</v>
+      <c r="B89" s="21" t="inlineStr">
+        <is>
+          <t>1/16/2025</t>
+        </is>
       </c>
       <c r="C89" s="22">
         <f>B89</f>
@@ -11769,7 +11945,7 @@
       </c>
       <c r="Y89" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z89" s="6" t="inlineStr">
@@ -11797,8 +11973,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B90" s="21" t="n">
-        <v>45678</v>
+      <c r="B90" s="21" t="inlineStr">
+        <is>
+          <t>1/21/2025</t>
+        </is>
       </c>
       <c r="C90" s="22">
         <f>B90</f>
@@ -11889,7 +12067,7 @@
       </c>
       <c r="Y90" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z90" s="6" t="inlineStr">
@@ -11917,8 +12095,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B91" s="21" t="n">
-        <v>45679</v>
+      <c r="B91" s="21" t="inlineStr">
+        <is>
+          <t>1/22/2025</t>
+        </is>
       </c>
       <c r="C91" s="22">
         <f>B91</f>
@@ -12009,7 +12189,7 @@
       </c>
       <c r="Y91" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z91" s="6" t="inlineStr">
@@ -12037,8 +12217,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B92" s="21" t="n">
-        <v>45680</v>
+      <c r="B92" s="21" t="inlineStr">
+        <is>
+          <t>1/23/2025</t>
+        </is>
       </c>
       <c r="C92" s="22">
         <f>B92</f>
@@ -12129,7 +12311,7 @@
       </c>
       <c r="Y92" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z92" s="6" t="inlineStr">
@@ -12157,8 +12339,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B93" s="21" t="n">
-        <v>45688</v>
+      <c r="B93" s="21" t="inlineStr">
+        <is>
+          <t>1/31/2025</t>
+        </is>
       </c>
       <c r="C93" s="22">
         <f>B93</f>
@@ -12249,7 +12433,7 @@
       </c>
       <c r="Y93" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z93" s="6" t="inlineStr">
@@ -12277,8 +12461,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B94" s="21" t="n">
-        <v>45686</v>
+      <c r="B94" s="21" t="inlineStr">
+        <is>
+          <t>1/29/2025</t>
+        </is>
       </c>
       <c r="C94" s="22">
         <f>B94</f>
@@ -12369,7 +12555,7 @@
       </c>
       <c r="Y94" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z94" s="6" t="inlineStr">
@@ -12397,8 +12583,10 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B95" s="21" t="n">
-        <v>45684</v>
+      <c r="B95" s="21" t="inlineStr">
+        <is>
+          <t>1/27/2025</t>
+        </is>
       </c>
       <c r="C95" s="22">
         <f>B95</f>
@@ -12489,7 +12677,7 @@
       </c>
       <c r="Y95" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z95" s="6" t="inlineStr">
@@ -12517,7 +12705,9 @@
           <t>A Partnership:Covered CA</t>
         </is>
       </c>
-      <c r="B96" s="21" t="n"/>
+      <c r="B96" s="21" t="n">
+        <v/>
+      </c>
       <c r="C96" s="22">
         <f>B96</f>
         <v/>
@@ -12601,7 +12791,7 @@
       </c>
       <c r="Y96" s="6" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Broadcast</t>
         </is>
       </c>
       <c r="Z96" s="6" t="inlineStr">

</xml_diff>